<commit_message>
Addig dplyr relational examples
</commit_message>
<xml_diff>
--- a/datasets/CSO/PopulationByProvince_1986_2016.xlsx
+++ b/datasets/CSO/PopulationByProvince_1986_2016.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimd/Dropbox/R Projects/CT5102/datasets/CSO/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D803DCB-30B2-C549-82DF-92C62E00E488}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PopulationByProvince1986-2016" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -51,16 +57,16 @@
     <t>Connacht</t>
   </si>
   <si>
-    <t>Ulster (part of)</t>
-  </si>
-  <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>Ulster</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -125,20 +131,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -150,6 +159,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -474,21 +491,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="2" max="4" width="10.83203125" style="5"/>
+    <col min="5" max="5" width="13" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
-        <v>11</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>7</v>
@@ -500,125 +518,125 @@
         <v>9</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>1852649</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>1020577</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="4">
         <v>431409</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="4">
         <v>236008</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>1860949</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>1009533</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <v>423031</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="4">
         <v>232206</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>1924702</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>1033903</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <v>433231</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <v>234251</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="4">
         <v>2105579</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>1100614</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <v>464296</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="4">
         <v>246714</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="4">
         <v>2295123</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <v>1173340</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="4">
         <v>504121</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="4">
         <v>267264</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="4">
         <v>2504814</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <v>1246088</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <v>542547</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="4">
         <v>294803</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="4">
         <v>2634403</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="4">
         <v>1280020</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="4">
         <v>550688</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="4">
         <v>296754</v>
       </c>
     </row>

</xml_diff>